<commit_message>
general updates for 2024-2025 season
I discovered this project a few days ago and I decided to update some information for the new season. I am not familiar at all neither with the neural network algorithm nor with TensorFlow, this is a purely amateur project.
</commit_message>
<xml_diff>
--- a/tmp/playermatchdata.xlsx
+++ b/tmp/playermatchdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="769">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -2311,16 +2311,13 @@
     <t>opp_vs_team_aerials_won_pct</t>
   </si>
   <si>
-    <t>Barella</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Inter</t>
-  </si>
-  <si>
-    <t>26-240</t>
+    <t>Immobile</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Lazio</t>
   </si>
   <si>
     <t>Atalanta</t>
@@ -4992,10 +4989,10 @@
         <v>765</v>
       </c>
       <c r="B2">
-        <v>269</v>
+        <v>450</v>
       </c>
       <c r="C2">
-        <v>1870</v>
+        <v>785</v>
       </c>
       <c r="D2" t="s">
         <v>766</v>
@@ -5007,172 +5004,172 @@
         <v>765</v>
       </c>
       <c r="H2">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>768</v>
+        <v>265</v>
+      </c>
+      <c r="I2">
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>1997</v>
+        <v>1990</v>
       </c>
       <c r="K2">
+        <v>31</v>
+      </c>
+      <c r="L2">
+        <v>21</v>
+      </c>
+      <c r="M2">
+        <v>1652</v>
+      </c>
+      <c r="N2">
         <v>7</v>
-      </c>
-      <c r="L2">
-        <v>6</v>
-      </c>
-      <c r="M2">
-        <v>476</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="U2">
-        <v>0.19</v>
+        <v>0.05</v>
       </c>
       <c r="V2">
-        <v>0.19</v>
+        <v>0.44</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="X2">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="Y2">
-        <v>0.3</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="Z2">
-        <v>0.3</v>
+        <v>6.6</v>
       </c>
       <c r="AA2">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
       <c r="AB2">
-        <v>0.05</v>
+        <v>0.36</v>
       </c>
       <c r="AC2">
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>14.3</v>
+        <v>42.2</v>
       </c>
       <c r="AG2">
-        <v>0.19</v>
+        <v>1.04</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="AJ2">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AK2">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="AL2">
-        <v>-0.3</v>
+        <v>-3.6</v>
       </c>
       <c r="AM2">
-        <v>298</v>
+        <v>338</v>
       </c>
       <c r="AN2">
-        <v>346</v>
+        <v>461</v>
       </c>
       <c r="AO2">
-        <v>86.09999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="AP2">
-        <v>4998</v>
+        <v>4444</v>
       </c>
       <c r="AQ2">
-        <v>1872</v>
+        <v>668</v>
       </c>
       <c r="AR2">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="AS2">
-        <v>169</v>
+        <v>268</v>
       </c>
       <c r="AT2">
-        <v>92.3</v>
+        <v>78.7</v>
       </c>
       <c r="AU2">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="AV2">
         <v>119</v>
       </c>
       <c r="AW2">
-        <v>89.09999999999999</v>
+        <v>77.3</v>
       </c>
       <c r="AX2">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="AY2">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="AZ2">
-        <v>55.6</v>
+        <v>61.9</v>
       </c>
       <c r="BA2">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="BB2">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="BC2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="BD2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="BF2">
-        <v>337</v>
+        <v>428</v>
       </c>
       <c r="BG2">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="BH2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BI2">
         <v>2</v>
       </c>
       <c r="BJ2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="BK2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BL2">
         <v>1</v>
@@ -5187,40 +5184,40 @@
         <v>0</v>
       </c>
       <c r="BP2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BQ2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BR2">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="BS2">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="BT2">
-        <v>4.16</v>
+        <v>2.18</v>
       </c>
       <c r="BU2">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="BV2">
         <v>0</v>
       </c>
       <c r="BW2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BX2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BY2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BZ2">
-        <v>0.57</v>
+        <v>0.22</v>
       </c>
       <c r="CA2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CB2">
         <v>0</v>
@@ -5229,100 +5226,100 @@
         <v>0</v>
       </c>
       <c r="CD2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CE2">
         <v>0</v>
       </c>
       <c r="CF2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="CG2">
+        <v>9</v>
+      </c>
+      <c r="CH2">
+        <v>2</v>
+      </c>
+      <c r="CI2">
+        <v>5</v>
+      </c>
+      <c r="CJ2">
+        <v>4</v>
+      </c>
+      <c r="CK2">
+        <v>9</v>
+      </c>
+      <c r="CL2">
+        <v>3</v>
+      </c>
+      <c r="CM2">
         <v>6</v>
       </c>
-      <c r="CH2">
-        <v>6</v>
-      </c>
-      <c r="CI2">
-        <v>6</v>
-      </c>
-      <c r="CJ2">
-        <v>1</v>
-      </c>
-      <c r="CK2">
-        <v>2</v>
-      </c>
-      <c r="CL2">
-        <v>0</v>
-      </c>
-      <c r="CM2">
-        <v>2</v>
-      </c>
       <c r="CN2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CO2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="CP2">
         <v>0</v>
       </c>
       <c r="CQ2">
-        <v>392</v>
+        <v>655</v>
       </c>
       <c r="CR2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="CS2">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="CT2">
-        <v>223</v>
+        <v>267</v>
       </c>
       <c r="CU2">
-        <v>113</v>
+        <v>350</v>
       </c>
       <c r="CV2">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="CW2">
-        <v>392</v>
+        <v>651</v>
       </c>
       <c r="CX2">
-        <v>240</v>
+        <v>327</v>
       </c>
       <c r="CY2">
+        <v>19</v>
+      </c>
+      <c r="CZ2">
+        <v>13</v>
+      </c>
+      <c r="DA2">
         <v>14</v>
       </c>
-      <c r="CZ2">
-        <v>8</v>
-      </c>
-      <c r="DA2">
-        <v>1</v>
-      </c>
       <c r="DB2">
-        <v>315</v>
+        <v>499</v>
       </c>
       <c r="DC2">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="DD2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="DE2">
         <v>0</v>
       </c>
       <c r="DF2">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="DG2">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="DH2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="DI2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DJ2">
         <v>0</v>
@@ -5331,16 +5328,16 @@
         <v>0</v>
       </c>
       <c r="DL2">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="DM2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="DN2">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="DO2">
-        <v>75</v>
+        <v>33.3</v>
       </c>
       <c r="DP2">
         <v>0</v>
@@ -5463,571 +5460,571 @@
         <v>0</v>
       </c>
       <c r="FD2">
-        <v>6.285714285714286</v>
+        <v>5.910714285714286</v>
       </c>
       <c r="FE2">
-        <v>0.4517539514526256</v>
+        <v>0.6131530254781927</v>
       </c>
       <c r="FF2" t="s">
         <v>767</v>
       </c>
       <c r="FG2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="FH2">
-        <v>54.7</v>
+        <v>53.3</v>
       </c>
       <c r="FI2">
+        <v>38</v>
+      </c>
+      <c r="FJ2">
+        <v>418</v>
+      </c>
+      <c r="FK2">
+        <v>3420</v>
+      </c>
+      <c r="FL2">
+        <v>46</v>
+      </c>
+      <c r="FM2">
+        <v>30</v>
+      </c>
+      <c r="FN2">
+        <v>4</v>
+      </c>
+      <c r="FO2">
+        <v>4</v>
+      </c>
+      <c r="FP2">
+        <v>101</v>
+      </c>
+      <c r="FQ2">
+        <v>5</v>
+      </c>
+      <c r="FR2">
+        <v>1.21</v>
+      </c>
+      <c r="FS2">
+        <v>0.79</v>
+      </c>
+      <c r="FT2">
+        <v>2</v>
+      </c>
+      <c r="FU2">
+        <v>1.11</v>
+      </c>
+      <c r="FV2">
+        <v>1.89</v>
+      </c>
+      <c r="FW2">
+        <v>46.5</v>
+      </c>
+      <c r="FX2">
+        <v>43.4</v>
+      </c>
+      <c r="FY2">
+        <v>1.22</v>
+      </c>
+      <c r="FZ2">
+        <v>1.14</v>
+      </c>
+      <c r="GA2">
+        <v>38</v>
+      </c>
+      <c r="GB2">
+        <v>38</v>
+      </c>
+      <c r="GC2">
+        <v>3420</v>
+      </c>
+      <c r="GD2">
+        <v>39</v>
+      </c>
+      <c r="GE2">
+        <v>1.03</v>
+      </c>
+      <c r="GF2">
+        <v>148</v>
+      </c>
+      <c r="GG2">
+        <v>109</v>
+      </c>
+      <c r="GH2">
+        <v>75</v>
+      </c>
+      <c r="GI2">
+        <v>18</v>
+      </c>
+      <c r="GJ2">
         <v>7</v>
       </c>
-      <c r="FJ2">
-        <v>77</v>
-      </c>
-      <c r="FK2">
-        <v>630</v>
-      </c>
-      <c r="FL2">
-        <v>19</v>
-      </c>
-      <c r="FM2">
-        <v>15</v>
-      </c>
-      <c r="FN2">
+      <c r="GK2">
+        <v>13</v>
+      </c>
+      <c r="GL2">
+        <v>13</v>
+      </c>
+      <c r="GM2">
+        <v>34.2</v>
+      </c>
+      <c r="GN2">
         <v>3</v>
       </c>
-      <c r="FO2">
-        <v>3</v>
-      </c>
-      <c r="FP2">
-        <v>8</v>
-      </c>
-      <c r="FQ2">
-        <v>0</v>
-      </c>
-      <c r="FR2">
-        <v>2.71</v>
-      </c>
-      <c r="FS2">
-        <v>2.14</v>
-      </c>
-      <c r="FT2">
-        <v>4.86</v>
-      </c>
-      <c r="FU2">
-        <v>2.29</v>
-      </c>
-      <c r="FV2">
-        <v>4.43</v>
-      </c>
-      <c r="FW2">
-        <v>14.8</v>
-      </c>
-      <c r="FX2">
-        <v>12.5</v>
-      </c>
-      <c r="FY2">
-        <v>2.11</v>
-      </c>
-      <c r="FZ2">
-        <v>1.78</v>
-      </c>
-      <c r="GA2">
-        <v>7</v>
-      </c>
-      <c r="GB2">
-        <v>7</v>
-      </c>
-      <c r="GC2">
-        <v>630</v>
-      </c>
-      <c r="GD2">
-        <v>3</v>
-      </c>
-      <c r="GE2">
-        <v>0.43</v>
-      </c>
-      <c r="GF2">
-        <v>18</v>
-      </c>
-      <c r="GG2">
-        <v>15</v>
-      </c>
-      <c r="GH2">
-        <v>83.3</v>
-      </c>
-      <c r="GI2">
-        <v>6</v>
-      </c>
-      <c r="GJ2">
-        <v>0</v>
-      </c>
-      <c r="GK2">
-        <v>1</v>
-      </c>
-      <c r="GL2">
-        <v>5</v>
-      </c>
-      <c r="GM2">
-        <v>71.40000000000001</v>
-      </c>
-      <c r="GN2">
-        <v>0</v>
-      </c>
       <c r="GO2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="GP2">
         <v>0</v>
       </c>
       <c r="GQ2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR2">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="GS2">
         <v>0</v>
       </c>
       <c r="GT2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="GU2">
         <v>0</v>
       </c>
       <c r="GV2">
-        <v>3.1</v>
+        <v>38.3</v>
       </c>
       <c r="GW2">
-        <v>0.17</v>
+        <v>0.24</v>
       </c>
       <c r="GX2">
+        <v>-0.7</v>
+      </c>
+      <c r="GY2">
+        <v>-0.02</v>
+      </c>
+      <c r="GZ2">
+        <v>139</v>
+      </c>
+      <c r="HA2">
+        <v>366</v>
+      </c>
+      <c r="HB2">
+        <v>38</v>
+      </c>
+      <c r="HC2">
+        <v>985</v>
+      </c>
+      <c r="HD2">
+        <v>132</v>
+      </c>
+      <c r="HE2">
+        <v>29.5</v>
+      </c>
+      <c r="HF2">
+        <v>37.7</v>
+      </c>
+      <c r="HG2">
+        <v>301</v>
+      </c>
+      <c r="HH2">
+        <v>24.9</v>
+      </c>
+      <c r="HI2">
+        <v>28.1</v>
+      </c>
+      <c r="HJ2">
+        <v>476</v>
+      </c>
+      <c r="HK2">
+        <v>21</v>
+      </c>
+      <c r="HL2">
+        <v>4.4</v>
+      </c>
+      <c r="HM2">
+        <v>23</v>
+      </c>
+      <c r="HN2">
+        <v>0.61</v>
+      </c>
+      <c r="HO2">
+        <v>13.1</v>
+      </c>
+      <c r="HP2">
+        <v>135</v>
+      </c>
+      <c r="HQ2">
+        <v>15</v>
+      </c>
+      <c r="HR2">
+        <v>31</v>
+      </c>
+      <c r="HS2">
+        <v>3.55</v>
+      </c>
+      <c r="HT2">
         <v>0.1</v>
       </c>
-      <c r="GY2">
-        <v>0.01</v>
-      </c>
-      <c r="GZ2">
-        <v>37</v>
-      </c>
-      <c r="HA2">
-        <v>66</v>
-      </c>
-      <c r="HB2">
-        <v>56.1</v>
-      </c>
-      <c r="HC2">
-        <v>202</v>
-      </c>
-      <c r="HD2">
-        <v>29</v>
-      </c>
-      <c r="HE2">
-        <v>28.2</v>
-      </c>
-      <c r="HF2">
-        <v>29.5</v>
-      </c>
-      <c r="HG2">
-        <v>47</v>
-      </c>
-      <c r="HH2">
-        <v>19.1</v>
-      </c>
-      <c r="HI2">
-        <v>25.8</v>
-      </c>
-      <c r="HJ2">
-        <v>65</v>
-      </c>
-      <c r="HK2">
-        <v>5</v>
-      </c>
-      <c r="HL2">
-        <v>7.7</v>
-      </c>
-      <c r="HM2">
-        <v>2</v>
-      </c>
-      <c r="HN2">
-        <v>0.29</v>
-      </c>
-      <c r="HO2">
-        <v>10</v>
-      </c>
-      <c r="HP2">
-        <v>35</v>
-      </c>
-      <c r="HQ2">
-        <v>4</v>
-      </c>
-      <c r="HR2">
-        <v>28.5</v>
-      </c>
-      <c r="HS2">
-        <v>5</v>
-      </c>
-      <c r="HT2">
-        <v>0.13</v>
-      </c>
       <c r="HU2">
-        <v>0.46</v>
+        <v>0.31</v>
       </c>
       <c r="HV2">
         <v>0.1</v>
       </c>
       <c r="HW2">
-        <v>4.2</v>
+        <v>-0.5</v>
       </c>
       <c r="HX2">
-        <v>3.5</v>
+        <v>-1.4</v>
       </c>
       <c r="HY2">
-        <v>3252</v>
+        <v>17462</v>
       </c>
       <c r="HZ2">
-        <v>3876</v>
+        <v>21071</v>
       </c>
       <c r="IA2">
-        <v>83.90000000000001</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="IB2">
-        <v>57107</v>
+        <v>293219</v>
       </c>
       <c r="IC2">
-        <v>20258</v>
+        <v>101247</v>
       </c>
       <c r="ID2">
-        <v>1488</v>
+        <v>8440</v>
       </c>
       <c r="IE2">
-        <v>1633</v>
+        <v>9314</v>
       </c>
       <c r="IF2">
-        <v>91.09999999999999</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="IG2">
-        <v>1292</v>
+        <v>6970</v>
       </c>
       <c r="IH2">
-        <v>1462</v>
+        <v>7966</v>
       </c>
       <c r="II2">
-        <v>88.40000000000001</v>
+        <v>87.5</v>
       </c>
       <c r="IJ2">
-        <v>345</v>
+        <v>1557</v>
       </c>
       <c r="IK2">
-        <v>544</v>
+        <v>2657</v>
       </c>
       <c r="IL2">
-        <v>63.4</v>
+        <v>58.6</v>
       </c>
       <c r="IM2">
-        <v>96</v>
+        <v>331</v>
       </c>
       <c r="IN2">
-        <v>232</v>
+        <v>1270</v>
       </c>
       <c r="IO2">
-        <v>92</v>
+        <v>316</v>
       </c>
       <c r="IP2">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="IQ2">
-        <v>308</v>
+        <v>1528</v>
       </c>
       <c r="IR2">
-        <v>3552</v>
+        <v>19202</v>
       </c>
       <c r="IS2">
-        <v>314</v>
+        <v>1797</v>
       </c>
       <c r="IT2">
-        <v>84</v>
+        <v>474</v>
       </c>
       <c r="IU2">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="IV2">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="IW2">
-        <v>154</v>
+        <v>624</v>
       </c>
       <c r="IX2">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="IY2">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="IZ2">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="JA2">
         <v>0</v>
       </c>
       <c r="JB2">
-        <v>134</v>
+        <v>748</v>
       </c>
       <c r="JC2">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="JD2">
-        <v>59</v>
+        <v>367</v>
       </c>
       <c r="JE2">
-        <v>227</v>
+        <v>762</v>
       </c>
       <c r="JF2">
-        <v>32.43</v>
+        <v>20.05</v>
       </c>
       <c r="JG2">
-        <v>181</v>
+        <v>573</v>
       </c>
       <c r="JH2">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="JI2">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="JJ2">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="JK2">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="JL2">
-        <v>4.86</v>
+        <v>1.95</v>
       </c>
       <c r="JM2">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="JN2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="JO2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="JP2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="JQ2">
         <v>1</v>
       </c>
       <c r="JR2">
-        <v>114</v>
+        <v>581</v>
       </c>
       <c r="JS2">
-        <v>67</v>
+        <v>348</v>
       </c>
       <c r="JT2">
-        <v>56</v>
+        <v>259</v>
       </c>
       <c r="JU2">
-        <v>48</v>
+        <v>254</v>
       </c>
       <c r="JV2">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="JW2">
-        <v>70</v>
+        <v>430</v>
       </c>
       <c r="JX2">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="JY2">
-        <v>46</v>
+        <v>308</v>
       </c>
       <c r="JZ2">
-        <v>57</v>
+        <v>295</v>
       </c>
       <c r="KA2">
-        <v>79</v>
+        <v>640</v>
       </c>
       <c r="KB2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="KC2">
-        <v>4548</v>
+        <v>24841</v>
       </c>
       <c r="KD2">
-        <v>408</v>
+        <v>2339</v>
       </c>
       <c r="KE2">
-        <v>1382</v>
+        <v>7512</v>
       </c>
       <c r="KF2">
-        <v>2028</v>
+        <v>12114</v>
       </c>
       <c r="KG2">
-        <v>1172</v>
+        <v>5447</v>
       </c>
       <c r="KH2">
-        <v>235</v>
+        <v>774</v>
       </c>
       <c r="KI2">
-        <v>4545</v>
+        <v>24837</v>
       </c>
       <c r="KJ2">
-        <v>2735</v>
+        <v>13267</v>
       </c>
       <c r="KK2">
+        <v>716</v>
+      </c>
+      <c r="KL2">
+        <v>521</v>
+      </c>
+      <c r="KM2">
         <v>143</v>
       </c>
-      <c r="KL2">
-        <v>104</v>
-      </c>
-      <c r="KM2">
-        <v>40</v>
-      </c>
       <c r="KN2">
-        <v>3221</v>
+        <v>17337</v>
       </c>
       <c r="KO2">
-        <v>81</v>
+        <v>507</v>
       </c>
       <c r="KP2">
-        <v>34</v>
+        <v>243</v>
       </c>
       <c r="KQ2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="KR2">
-        <v>78</v>
+        <v>473</v>
       </c>
       <c r="KS2">
-        <v>79</v>
+        <v>435</v>
       </c>
       <c r="KT2">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="KU2">
         <v>3</v>
       </c>
       <c r="KV2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="KW2">
         <v>0</v>
       </c>
       <c r="KX2">
-        <v>324</v>
+        <v>1764</v>
       </c>
       <c r="KY2">
-        <v>108</v>
+        <v>399</v>
       </c>
       <c r="KZ2">
-        <v>57</v>
+        <v>453</v>
       </c>
       <c r="LA2">
-        <v>65.5</v>
+        <v>46.8</v>
       </c>
       <c r="LB2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="LC2">
-        <v>45.3</v>
+        <v>46.7</v>
       </c>
       <c r="LD2">
+        <v>38</v>
+      </c>
+      <c r="LE2">
+        <v>418</v>
+      </c>
+      <c r="LF2">
+        <v>3420</v>
+      </c>
+      <c r="LG2">
+        <v>39</v>
+      </c>
+      <c r="LH2">
+        <v>27</v>
+      </c>
+      <c r="LI2">
+        <v>2</v>
+      </c>
+      <c r="LJ2">
+        <v>3</v>
+      </c>
+      <c r="LK2">
+        <v>95</v>
+      </c>
+      <c r="LL2">
+        <v>3</v>
+      </c>
+      <c r="LM2">
+        <v>1.03</v>
+      </c>
+      <c r="LN2">
+        <v>0.71</v>
+      </c>
+      <c r="LO2">
+        <v>1.74</v>
+      </c>
+      <c r="LP2">
+        <v>0.97</v>
+      </c>
+      <c r="LQ2">
+        <v>1.68</v>
+      </c>
+      <c r="LR2">
+        <v>42</v>
+      </c>
+      <c r="LS2">
+        <v>39.6</v>
+      </c>
+      <c r="LT2">
+        <v>1.11</v>
+      </c>
+      <c r="LU2">
+        <v>1.04</v>
+      </c>
+      <c r="LV2">
+        <v>38</v>
+      </c>
+      <c r="LW2">
+        <v>38</v>
+      </c>
+      <c r="LX2">
+        <v>3420</v>
+      </c>
+      <c r="LY2">
+        <v>49</v>
+      </c>
+      <c r="LZ2">
+        <v>1.29</v>
+      </c>
+      <c r="MA2">
+        <v>139</v>
+      </c>
+      <c r="MB2">
+        <v>93</v>
+      </c>
+      <c r="MC2">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="MD2">
+        <v>13</v>
+      </c>
+      <c r="ME2">
         <v>7</v>
       </c>
-      <c r="LE2">
-        <v>77</v>
-      </c>
-      <c r="LF2">
-        <v>630</v>
-      </c>
-      <c r="LG2">
-        <v>3</v>
-      </c>
-      <c r="LH2">
-        <v>3</v>
-      </c>
-      <c r="LI2">
-        <v>0</v>
-      </c>
-      <c r="LJ2">
-        <v>0</v>
-      </c>
-      <c r="LK2">
-        <v>10</v>
-      </c>
-      <c r="LL2">
-        <v>0</v>
-      </c>
-      <c r="LM2">
-        <v>0.43</v>
-      </c>
-      <c r="LN2">
-        <v>0.43</v>
-      </c>
-      <c r="LO2">
-        <v>0.86</v>
-      </c>
-      <c r="LP2">
-        <v>0.43</v>
-      </c>
-      <c r="LQ2">
-        <v>0.86</v>
-      </c>
-      <c r="LR2">
-        <v>4.8</v>
-      </c>
-      <c r="LS2">
-        <v>4.8</v>
-      </c>
-      <c r="LT2">
-        <v>0.68</v>
-      </c>
-      <c r="LU2">
-        <v>0.68</v>
-      </c>
-      <c r="LV2">
-        <v>7</v>
-      </c>
-      <c r="LW2">
-        <v>7</v>
-      </c>
-      <c r="LX2">
-        <v>630</v>
-      </c>
-      <c r="LY2">
-        <v>19</v>
-      </c>
-      <c r="LZ2">
-        <v>2.71</v>
-      </c>
-      <c r="MA2">
-        <v>38</v>
-      </c>
-      <c r="MB2">
-        <v>19</v>
-      </c>
-      <c r="MC2">
-        <v>57.9</v>
-      </c>
-      <c r="MD2">
-        <v>1</v>
-      </c>
-      <c r="ME2">
-        <v>0</v>
-      </c>
       <c r="MF2">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="MG2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="MH2">
-        <v>0</v>
+        <v>21.1</v>
       </c>
       <c r="MI2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="MJ2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="MK2">
         <v>0</v>
@@ -6036,547 +6033,547 @@
         <v>0</v>
       </c>
       <c r="MM2">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="MN2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="MO2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="MP2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="MQ2">
-        <v>13.6</v>
+        <v>46.7</v>
       </c>
       <c r="MR2">
-        <v>0.29</v>
+        <v>0.31</v>
       </c>
       <c r="MS2">
-        <v>-5.4</v>
+        <v>0.7</v>
       </c>
       <c r="MT2">
-        <v>-0.77</v>
+        <v>0.02</v>
       </c>
       <c r="MU2">
+        <v>219</v>
+      </c>
+      <c r="MV2">
+        <v>486</v>
+      </c>
+      <c r="MW2">
+        <v>45.1</v>
+      </c>
+      <c r="MX2">
+        <v>1206</v>
+      </c>
+      <c r="MY2">
+        <v>185</v>
+      </c>
+      <c r="MZ2">
+        <v>30.1</v>
+      </c>
+      <c r="NA2">
+        <v>30.7</v>
+      </c>
+      <c r="NB2">
+        <v>281</v>
+      </c>
+      <c r="NC2">
+        <v>43.8</v>
+      </c>
+      <c r="ND2">
+        <v>38.8</v>
+      </c>
+      <c r="NE2">
+        <v>490</v>
+      </c>
+      <c r="NF2">
+        <v>21</v>
+      </c>
+      <c r="NG2">
+        <v>4.3</v>
+      </c>
+      <c r="NH2">
         <v>30</v>
       </c>
-      <c r="MV2">
-        <v>99</v>
-      </c>
-      <c r="MW2">
-        <v>30.3</v>
-      </c>
-      <c r="MX2">
-        <v>193</v>
-      </c>
-      <c r="MY2">
-        <v>31</v>
-      </c>
-      <c r="MZ2">
-        <v>35.8</v>
-      </c>
-      <c r="NA2">
-        <v>34.8</v>
-      </c>
-      <c r="NB2">
-        <v>51</v>
-      </c>
-      <c r="NC2">
-        <v>58.8</v>
-      </c>
-      <c r="ND2">
-        <v>46.6</v>
-      </c>
-      <c r="NE2">
-        <v>117</v>
-      </c>
-      <c r="NF2">
-        <v>2</v>
-      </c>
-      <c r="NG2">
-        <v>1.7</v>
-      </c>
-      <c r="NH2">
-        <v>5</v>
-      </c>
       <c r="NI2">
-        <v>0.71</v>
+        <v>0.79</v>
       </c>
       <c r="NJ2">
-        <v>11.6</v>
+        <v>13.1</v>
       </c>
       <c r="NK2">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="NL2">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="NM2">
-        <v>25.4</v>
+        <v>30.2</v>
       </c>
       <c r="NN2">
-        <v>2.57</v>
+        <v>3.84</v>
       </c>
       <c r="NO2">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="NP2">
-        <v>0.17</v>
+        <v>0.25</v>
       </c>
       <c r="NQ2">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="NR2">
-        <v>-1.8</v>
+        <v>-3</v>
       </c>
       <c r="NS2">
-        <v>-1.8</v>
+        <v>-2.6</v>
       </c>
       <c r="NT2">
-        <v>2613</v>
+        <v>15117</v>
       </c>
       <c r="NU2">
-        <v>3177</v>
+        <v>18552</v>
       </c>
       <c r="NV2">
-        <v>82.2</v>
+        <v>81.5</v>
       </c>
       <c r="NW2">
-        <v>46995</v>
+        <v>275979</v>
       </c>
       <c r="NX2">
-        <v>15906</v>
+        <v>93061</v>
       </c>
       <c r="NY2">
-        <v>1147</v>
+        <v>6158</v>
       </c>
       <c r="NZ2">
-        <v>1280</v>
+        <v>6936</v>
       </c>
       <c r="OA2">
-        <v>89.59999999999999</v>
+        <v>88.8</v>
       </c>
       <c r="OB2">
-        <v>1105</v>
+        <v>7030</v>
       </c>
       <c r="OC2">
-        <v>1245</v>
+        <v>7918</v>
       </c>
       <c r="OD2">
         <v>88.8</v>
       </c>
       <c r="OE2">
-        <v>288</v>
+        <v>1557</v>
       </c>
       <c r="OF2">
-        <v>476</v>
+        <v>2760</v>
       </c>
       <c r="OG2">
-        <v>60.5</v>
+        <v>56.4</v>
       </c>
       <c r="OH2">
-        <v>56</v>
+        <v>365</v>
       </c>
       <c r="OI2">
-        <v>190</v>
+        <v>913</v>
       </c>
       <c r="OJ2">
-        <v>56</v>
+        <v>253</v>
       </c>
       <c r="OK2">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="OL2">
-        <v>236</v>
+        <v>1169</v>
       </c>
       <c r="OM2">
-        <v>2863</v>
+        <v>16735</v>
       </c>
       <c r="ON2">
-        <v>303</v>
+        <v>1778</v>
       </c>
       <c r="OO2">
-        <v>84</v>
+        <v>519</v>
       </c>
       <c r="OP2">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="OQ2">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="OR2">
-        <v>95</v>
+        <v>614</v>
       </c>
       <c r="OS2">
-        <v>20</v>
+        <v>174</v>
       </c>
       <c r="OT2">
+        <v>54</v>
+      </c>
+      <c r="OU2">
+        <v>76</v>
+      </c>
+      <c r="OV2">
+        <v>1</v>
+      </c>
+      <c r="OW2">
+        <v>719</v>
+      </c>
+      <c r="OX2">
+        <v>39</v>
+      </c>
+      <c r="OY2">
+        <v>349</v>
+      </c>
+      <c r="OZ2">
+        <v>868</v>
+      </c>
+      <c r="PA2">
+        <v>22.84</v>
+      </c>
+      <c r="PB2">
+        <v>603</v>
+      </c>
+      <c r="PC2">
+        <v>92</v>
+      </c>
+      <c r="PD2">
+        <v>69</v>
+      </c>
+      <c r="PE2">
+        <v>47</v>
+      </c>
+      <c r="PF2">
+        <v>64</v>
+      </c>
+      <c r="PG2">
+        <v>1.68</v>
+      </c>
+      <c r="PH2">
+        <v>43</v>
+      </c>
+      <c r="PI2">
         <v>7</v>
       </c>
-      <c r="OU2">
-        <v>10</v>
-      </c>
-      <c r="OV2">
-        <v>0</v>
-      </c>
-      <c r="OW2">
-        <v>108</v>
-      </c>
-      <c r="OX2">
-        <v>11</v>
-      </c>
-      <c r="OY2">
-        <v>60</v>
-      </c>
-      <c r="OZ2">
-        <v>123</v>
-      </c>
-      <c r="PA2">
-        <v>17.57</v>
-      </c>
-      <c r="PB2">
-        <v>102</v>
-      </c>
-      <c r="PC2">
+      <c r="PJ2">
+        <v>8</v>
+      </c>
+      <c r="PK2">
         <v>4</v>
-      </c>
-      <c r="PD2">
-        <v>2</v>
-      </c>
-      <c r="PE2">
-        <v>5</v>
-      </c>
-      <c r="PF2">
-        <v>6</v>
-      </c>
-      <c r="PG2">
-        <v>0.86</v>
-      </c>
-      <c r="PH2">
-        <v>6</v>
-      </c>
-      <c r="PI2">
-        <v>0</v>
-      </c>
-      <c r="PJ2">
-        <v>0</v>
-      </c>
-      <c r="PK2">
-        <v>0</v>
       </c>
       <c r="PL2">
         <v>0</v>
       </c>
       <c r="PM2">
-        <v>69</v>
+        <v>512</v>
       </c>
       <c r="PN2">
-        <v>43</v>
+        <v>303</v>
       </c>
       <c r="PO2">
-        <v>35</v>
+        <v>239</v>
       </c>
       <c r="PP2">
-        <v>26</v>
+        <v>211</v>
       </c>
       <c r="PQ2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="PR2">
-        <v>80</v>
+        <v>441</v>
       </c>
       <c r="PS2">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="PT2">
-        <v>46</v>
+        <v>319</v>
       </c>
       <c r="PU2">
-        <v>54</v>
+        <v>318</v>
       </c>
       <c r="PV2">
-        <v>159</v>
+        <v>702</v>
       </c>
       <c r="PW2">
+        <v>16</v>
+      </c>
+      <c r="PX2">
+        <v>22499</v>
+      </c>
+      <c r="PY2">
+        <v>2682</v>
+      </c>
+      <c r="PZ2">
+        <v>8716</v>
+      </c>
+      <c r="QA2">
+        <v>9527</v>
+      </c>
+      <c r="QB2">
+        <v>4462</v>
+      </c>
+      <c r="QC2">
+        <v>695</v>
+      </c>
+      <c r="QD2">
+        <v>22496</v>
+      </c>
+      <c r="QE2">
+        <v>13358</v>
+      </c>
+      <c r="QF2">
+        <v>601</v>
+      </c>
+      <c r="QG2">
+        <v>414</v>
+      </c>
+      <c r="QH2">
+        <v>145</v>
+      </c>
+      <c r="QI2">
+        <v>14997</v>
+      </c>
+      <c r="QJ2">
+        <v>547</v>
+      </c>
+      <c r="QK2">
+        <v>298</v>
+      </c>
+      <c r="QL2">
         <v>2</v>
       </c>
-      <c r="PX2">
-        <v>3873</v>
-      </c>
-      <c r="PY2">
-        <v>513</v>
-      </c>
-      <c r="PZ2">
-        <v>1258</v>
-      </c>
-      <c r="QA2">
-        <v>1778</v>
-      </c>
-      <c r="QB2">
-        <v>873</v>
-      </c>
-      <c r="QC2">
-        <v>118</v>
-      </c>
-      <c r="QD2">
-        <v>3873</v>
-      </c>
-      <c r="QE2">
-        <v>2419</v>
-      </c>
-      <c r="QF2">
-        <v>132</v>
-      </c>
-      <c r="QG2">
-        <v>97</v>
-      </c>
-      <c r="QH2">
-        <v>24</v>
-      </c>
-      <c r="QI2">
-        <v>2586</v>
-      </c>
-      <c r="QJ2">
+      <c r="QM2">
+        <v>459</v>
+      </c>
+      <c r="QN2">
+        <v>453</v>
+      </c>
+      <c r="QO2">
+        <v>39</v>
+      </c>
+      <c r="QP2">
+        <v>1</v>
+      </c>
+      <c r="QQ2">
+        <v>4</v>
+      </c>
+      <c r="QR2">
+        <v>3</v>
+      </c>
+      <c r="QS2">
+        <v>1782</v>
+      </c>
+      <c r="QT2">
+        <v>453</v>
+      </c>
+      <c r="QU2">
+        <v>399</v>
+      </c>
+      <c r="QV2">
+        <v>53.2</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>768</v>
+      </c>
+      <c r="QX2">
+        <v>29</v>
+      </c>
+      <c r="QY2">
+        <v>51.1</v>
+      </c>
+      <c r="QZ2">
+        <v>38</v>
+      </c>
+      <c r="RA2">
+        <v>418</v>
+      </c>
+      <c r="RB2">
+        <v>3420</v>
+      </c>
+      <c r="RC2">
+        <v>72</v>
+      </c>
+      <c r="RD2">
+        <v>57</v>
+      </c>
+      <c r="RE2">
+        <v>5</v>
+      </c>
+      <c r="RF2">
+        <v>5</v>
+      </c>
+      <c r="RG2">
+        <v>76</v>
+      </c>
+      <c r="RH2">
+        <v>1</v>
+      </c>
+      <c r="RI2">
+        <v>1.89</v>
+      </c>
+      <c r="RJ2">
+        <v>1.5</v>
+      </c>
+      <c r="RK2">
+        <v>3.39</v>
+      </c>
+      <c r="RL2">
+        <v>1.76</v>
+      </c>
+      <c r="RM2">
+        <v>3.26</v>
+      </c>
+      <c r="RN2">
+        <v>57.8</v>
+      </c>
+      <c r="RO2">
+        <v>53.9</v>
+      </c>
+      <c r="RP2">
+        <v>1.52</v>
+      </c>
+      <c r="RQ2">
+        <v>1.42</v>
+      </c>
+      <c r="RR2">
+        <v>38</v>
+      </c>
+      <c r="RS2">
+        <v>38</v>
+      </c>
+      <c r="RT2">
+        <v>3420</v>
+      </c>
+      <c r="RU2">
+        <v>42</v>
+      </c>
+      <c r="RV2">
+        <v>1.11</v>
+      </c>
+      <c r="RW2">
+        <v>142</v>
+      </c>
+      <c r="RX2">
         <v>99</v>
       </c>
-      <c r="QK2">
-        <v>62</v>
-      </c>
-      <c r="QL2">
-        <v>0</v>
-      </c>
-      <c r="QM2">
-        <v>82</v>
-      </c>
-      <c r="QN2">
-        <v>74</v>
-      </c>
-      <c r="QO2">
+      <c r="RY2">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="RZ2">
+        <v>21</v>
+      </c>
+      <c r="SA2">
+        <v>6</v>
+      </c>
+      <c r="SB2">
         <v>11</v>
       </c>
-      <c r="QP2">
-        <v>0</v>
-      </c>
-      <c r="QQ2">
-        <v>3</v>
-      </c>
-      <c r="QR2">
-        <v>0</v>
-      </c>
-      <c r="QS2">
-        <v>298</v>
-      </c>
-      <c r="QT2">
-        <v>57</v>
-      </c>
-      <c r="QU2">
-        <v>108</v>
-      </c>
-      <c r="QV2">
-        <v>34.5</v>
-      </c>
-      <c r="QW2" t="s">
-        <v>769</v>
-      </c>
-      <c r="QX2">
-        <v>24</v>
-      </c>
-      <c r="QY2">
-        <v>50.7</v>
-      </c>
-      <c r="QZ2">
-        <v>7</v>
-      </c>
-      <c r="RA2">
-        <v>77</v>
-      </c>
-      <c r="RB2">
-        <v>630</v>
-      </c>
-      <c r="RC2">
-        <v>11</v>
-      </c>
-      <c r="RD2">
-        <v>11</v>
-      </c>
-      <c r="RE2">
-        <v>0</v>
-      </c>
-      <c r="RF2">
-        <v>0</v>
-      </c>
-      <c r="RG2">
-        <v>10</v>
-      </c>
-      <c r="RH2">
-        <v>0</v>
-      </c>
-      <c r="RI2">
-        <v>1.57</v>
-      </c>
-      <c r="RJ2">
-        <v>1.57</v>
-      </c>
-      <c r="RK2">
-        <v>3.14</v>
-      </c>
-      <c r="RL2">
-        <v>1.57</v>
-      </c>
-      <c r="RM2">
-        <v>3.14</v>
-      </c>
-      <c r="RN2">
-        <v>9.1</v>
-      </c>
-      <c r="RO2">
-        <v>9.1</v>
-      </c>
-      <c r="RP2">
-        <v>1.3</v>
-      </c>
-      <c r="RQ2">
-        <v>1.3</v>
-      </c>
-      <c r="RR2">
-        <v>7</v>
-      </c>
-      <c r="RS2">
-        <v>7</v>
-      </c>
-      <c r="RT2">
-        <v>630</v>
-      </c>
-      <c r="RU2">
-        <v>5</v>
-      </c>
-      <c r="RV2">
-        <v>0.71</v>
-      </c>
-      <c r="RW2">
-        <v>23</v>
-      </c>
-      <c r="RX2">
-        <v>18</v>
-      </c>
-      <c r="RY2">
-        <v>78.3</v>
-      </c>
-      <c r="RZ2">
-        <v>4</v>
-      </c>
-      <c r="SA2">
+      <c r="SC2">
+        <v>15</v>
+      </c>
+      <c r="SD2">
+        <v>39.5</v>
+      </c>
+      <c r="SE2">
+        <v>9</v>
+      </c>
+      <c r="SF2">
+        <v>6</v>
+      </c>
+      <c r="SG2">
+        <v>2</v>
+      </c>
+      <c r="SH2">
         <v>1</v>
       </c>
-      <c r="SB2">
-        <v>2</v>
-      </c>
-      <c r="SC2">
-        <v>5</v>
-      </c>
-      <c r="SD2">
-        <v>71.40000000000001</v>
-      </c>
-      <c r="SE2">
-        <v>0</v>
-      </c>
-      <c r="SF2">
-        <v>0</v>
-      </c>
-      <c r="SG2">
-        <v>0</v>
-      </c>
-      <c r="SH2">
-        <v>0</v>
-      </c>
       <c r="SI2">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="SJ2">
         <v>0</v>
       </c>
       <c r="SK2">
+        <v>4</v>
+      </c>
+      <c r="SL2">
         <v>1</v>
       </c>
-      <c r="SL2">
-        <v>0</v>
-      </c>
       <c r="SM2">
-        <v>4.5</v>
+        <v>39.8</v>
       </c>
       <c r="SN2">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="SO2">
-        <v>-0.5</v>
+        <v>-1.2</v>
       </c>
       <c r="SP2">
-        <v>-0.07000000000000001</v>
+        <v>-0.03</v>
       </c>
       <c r="SQ2">
-        <v>22</v>
+        <v>161</v>
       </c>
       <c r="SR2">
-        <v>89</v>
+        <v>459</v>
       </c>
       <c r="SS2">
-        <v>24.7</v>
+        <v>35.1</v>
       </c>
       <c r="ST2">
+        <v>974</v>
+      </c>
+      <c r="SU2">
+        <v>213</v>
+      </c>
+      <c r="SV2">
+        <v>28.9</v>
+      </c>
+      <c r="SW2">
+        <v>29.6</v>
+      </c>
+      <c r="SX2">
+        <v>270</v>
+      </c>
+      <c r="SY2">
+        <v>65.90000000000001</v>
+      </c>
+      <c r="SZ2">
+        <v>50.1</v>
+      </c>
+      <c r="TA2">
+        <v>444</v>
+      </c>
+      <c r="TB2">
+        <v>30</v>
+      </c>
+      <c r="TC2">
+        <v>6.8</v>
+      </c>
+      <c r="TD2">
+        <v>55</v>
+      </c>
+      <c r="TE2">
+        <v>1.45</v>
+      </c>
+      <c r="TF2">
+        <v>16.7</v>
+      </c>
+      <c r="TG2">
         <v>197</v>
       </c>
-      <c r="SU2">
-        <v>43</v>
-      </c>
-      <c r="SV2">
-        <v>29.9</v>
-      </c>
-      <c r="SW2">
-        <v>31.6</v>
-      </c>
-      <c r="SX2">
-        <v>45</v>
-      </c>
-      <c r="SY2">
-        <v>66.7</v>
-      </c>
-      <c r="SZ2">
-        <v>51.7</v>
-      </c>
-      <c r="TA2">
-        <v>78</v>
-      </c>
-      <c r="TB2">
-        <v>8</v>
-      </c>
-      <c r="TC2">
-        <v>10.3</v>
-      </c>
-      <c r="TD2">
-        <v>12</v>
-      </c>
-      <c r="TE2">
-        <v>1.71</v>
-      </c>
-      <c r="TF2">
-        <v>18.1</v>
-      </c>
-      <c r="TG2">
-        <v>32</v>
-      </c>
       <c r="TH2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="TI2">
-        <v>33.3</v>
+        <v>36.5</v>
       </c>
       <c r="TJ2">
-        <v>4.57</v>
+        <v>5.18</v>
       </c>
       <c r="TK2">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="TL2">
         <v>0.34</v>
@@ -6585,358 +6582,358 @@
         <v>0.1</v>
       </c>
       <c r="TN2">
-        <v>1.9</v>
+        <v>14.2</v>
       </c>
       <c r="TO2">
-        <v>1.9</v>
+        <v>13.1</v>
       </c>
       <c r="TP2">
-        <v>2966</v>
+        <v>16051</v>
       </c>
       <c r="TQ2">
-        <v>3733</v>
+        <v>19961</v>
       </c>
       <c r="TR2">
-        <v>79.5</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="TS2">
-        <v>50437</v>
+        <v>281418</v>
       </c>
       <c r="TT2">
-        <v>17744</v>
+        <v>100413</v>
       </c>
       <c r="TU2">
-        <v>1392</v>
+        <v>7280</v>
       </c>
       <c r="TV2">
-        <v>1592</v>
+        <v>8321</v>
       </c>
       <c r="TW2">
-        <v>87.40000000000001</v>
+        <v>87.5</v>
       </c>
       <c r="TX2">
-        <v>1213</v>
+        <v>6956</v>
       </c>
       <c r="TY2">
-        <v>1403</v>
+        <v>7989</v>
       </c>
       <c r="TZ2">
-        <v>86.5</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="UA2">
-        <v>271</v>
+        <v>1466</v>
       </c>
       <c r="UB2">
-        <v>506</v>
+        <v>2642</v>
       </c>
       <c r="UC2">
-        <v>53.6</v>
+        <v>55.5</v>
       </c>
       <c r="UD2">
-        <v>73</v>
+        <v>437</v>
       </c>
       <c r="UE2">
-        <v>205</v>
+        <v>1223</v>
       </c>
       <c r="UF2">
+        <v>381</v>
+      </c>
+      <c r="UG2">
+        <v>114</v>
+      </c>
+      <c r="UH2">
+        <v>1754</v>
+      </c>
+      <c r="UI2">
+        <v>18129</v>
+      </c>
+      <c r="UJ2">
+        <v>1769</v>
+      </c>
+      <c r="UK2">
+        <v>439</v>
+      </c>
+      <c r="UL2">
+        <v>42</v>
+      </c>
+      <c r="UM2">
+        <v>124</v>
+      </c>
+      <c r="UN2">
+        <v>710</v>
+      </c>
+      <c r="UO2">
+        <v>210</v>
+      </c>
+      <c r="UP2">
+        <v>103</v>
+      </c>
+      <c r="UQ2">
         <v>67</v>
-      </c>
-      <c r="UG2">
-        <v>15</v>
-      </c>
-      <c r="UH2">
-        <v>315</v>
-      </c>
-      <c r="UI2">
-        <v>3397</v>
-      </c>
-      <c r="UJ2">
-        <v>319</v>
-      </c>
-      <c r="UK2">
-        <v>68</v>
-      </c>
-      <c r="UL2">
-        <v>9</v>
-      </c>
-      <c r="UM2">
-        <v>27</v>
-      </c>
-      <c r="UN2">
-        <v>130</v>
-      </c>
-      <c r="UO2">
-        <v>38</v>
-      </c>
-      <c r="UP2">
-        <v>14</v>
-      </c>
-      <c r="UQ2">
-        <v>15</v>
       </c>
       <c r="UR2">
         <v>1</v>
       </c>
       <c r="US2">
-        <v>156</v>
+        <v>772</v>
       </c>
       <c r="UT2">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="UU2">
-        <v>76</v>
+        <v>382</v>
       </c>
       <c r="UV2">
+        <v>971</v>
+      </c>
+      <c r="UW2">
+        <v>25.55</v>
+      </c>
+      <c r="UX2">
+        <v>735</v>
+      </c>
+      <c r="UY2">
+        <v>80</v>
+      </c>
+      <c r="UZ2">
+        <v>55</v>
+      </c>
+      <c r="VA2">
+        <v>32</v>
+      </c>
+      <c r="VB2">
+        <v>128</v>
+      </c>
+      <c r="VC2">
+        <v>3.37</v>
+      </c>
+      <c r="VD2">
+        <v>103</v>
+      </c>
+      <c r="VE2">
+        <v>9</v>
+      </c>
+      <c r="VF2">
+        <v>7</v>
+      </c>
+      <c r="VG2">
+        <v>6</v>
+      </c>
+      <c r="VH2">
+        <v>1</v>
+      </c>
+      <c r="VI2">
+        <v>613</v>
+      </c>
+      <c r="VJ2">
+        <v>369</v>
+      </c>
+      <c r="VK2">
+        <v>273</v>
+      </c>
+      <c r="VL2">
+        <v>249</v>
+      </c>
+      <c r="VM2">
+        <v>91</v>
+      </c>
+      <c r="VN2">
+        <v>483</v>
+      </c>
+      <c r="VO2">
+        <v>119</v>
+      </c>
+      <c r="VP2">
+        <v>364</v>
+      </c>
+      <c r="VQ2">
+        <v>340</v>
+      </c>
+      <c r="VR2">
+        <v>614</v>
+      </c>
+      <c r="VS2">
+        <v>7</v>
+      </c>
+      <c r="VT2">
+        <v>24136</v>
+      </c>
+      <c r="VU2">
+        <v>2222</v>
+      </c>
+      <c r="VV2">
+        <v>7494</v>
+      </c>
+      <c r="VW2">
+        <v>10658</v>
+      </c>
+      <c r="VX2">
+        <v>6186</v>
+      </c>
+      <c r="VY2">
+        <v>912</v>
+      </c>
+      <c r="VZ2">
+        <v>24131</v>
+      </c>
+      <c r="WA2">
+        <v>13093</v>
+      </c>
+      <c r="WB2">
+        <v>715</v>
+      </c>
+      <c r="WC2">
+        <v>519</v>
+      </c>
+      <c r="WD2">
         <v>175</v>
       </c>
-      <c r="UW2">
-        <v>25</v>
-      </c>
-      <c r="UX2">
-        <v>133</v>
-      </c>
-      <c r="UY2">
-        <v>13</v>
-      </c>
-      <c r="UZ2">
-        <v>10</v>
-      </c>
-      <c r="VA2">
-        <v>3</v>
-      </c>
-      <c r="VB2">
+      <c r="WE2">
+        <v>15915</v>
+      </c>
+      <c r="WF2">
+        <v>621</v>
+      </c>
+      <c r="WG2">
+        <v>377</v>
+      </c>
+      <c r="WH2">
+        <v>1</v>
+      </c>
+      <c r="WI2">
+        <v>486</v>
+      </c>
+      <c r="WJ2">
+        <v>367</v>
+      </c>
+      <c r="WK2">
+        <v>63</v>
+      </c>
+      <c r="WL2">
+        <v>4</v>
+      </c>
+      <c r="WM2">
+        <v>9</v>
+      </c>
+      <c r="WN2">
+        <v>1</v>
+      </c>
+      <c r="WO2">
+        <v>2023</v>
+      </c>
+      <c r="WP2">
+        <v>627</v>
+      </c>
+      <c r="WQ2">
+        <v>491</v>
+      </c>
+      <c r="WR2">
+        <v>56.1</v>
+      </c>
+      <c r="WS2">
+        <v>29</v>
+      </c>
+      <c r="WT2">
+        <v>48.9</v>
+      </c>
+      <c r="WU2">
+        <v>38</v>
+      </c>
+      <c r="WV2">
+        <v>418</v>
+      </c>
+      <c r="WW2">
+        <v>3420</v>
+      </c>
+      <c r="WX2">
+        <v>41</v>
+      </c>
+      <c r="WY2">
+        <v>32</v>
+      </c>
+      <c r="WZ2">
+        <v>6</v>
+      </c>
+      <c r="XA2">
+        <v>9</v>
+      </c>
+      <c r="XB2">
+        <v>67</v>
+      </c>
+      <c r="XC2">
+        <v>1</v>
+      </c>
+      <c r="XD2">
+        <v>1.08</v>
+      </c>
+      <c r="XE2">
+        <v>0.84</v>
+      </c>
+      <c r="XF2">
+        <v>1.92</v>
+      </c>
+      <c r="XG2">
+        <v>0.92</v>
+      </c>
+      <c r="XH2">
+        <v>1.76</v>
+      </c>
+      <c r="XI2">
+        <v>41.1</v>
+      </c>
+      <c r="XJ2">
+        <v>34.1</v>
+      </c>
+      <c r="XK2">
+        <v>1.08</v>
+      </c>
+      <c r="XL2">
+        <v>0.9</v>
+      </c>
+      <c r="XM2">
+        <v>38</v>
+      </c>
+      <c r="XN2">
+        <v>38</v>
+      </c>
+      <c r="XO2">
+        <v>3420</v>
+      </c>
+      <c r="XP2">
+        <v>72</v>
+      </c>
+      <c r="XQ2">
+        <v>1.89</v>
+      </c>
+      <c r="XR2">
+        <v>202</v>
+      </c>
+      <c r="XS2">
+        <v>130</v>
+      </c>
+      <c r="XT2">
+        <v>66.8</v>
+      </c>
+      <c r="XU2">
+        <v>11</v>
+      </c>
+      <c r="XV2">
+        <v>6</v>
+      </c>
+      <c r="XW2">
         <v>21</v>
       </c>
-      <c r="VC2">
-        <v>3</v>
-      </c>
-      <c r="VD2">
-        <v>19</v>
-      </c>
-      <c r="VE2">
-        <v>1</v>
-      </c>
-      <c r="VF2">
-        <v>1</v>
-      </c>
-      <c r="VG2">
-        <v>0</v>
-      </c>
-      <c r="VH2">
-        <v>0</v>
-      </c>
-      <c r="VI2">
-        <v>117</v>
-      </c>
-      <c r="VJ2">
-        <v>61</v>
-      </c>
-      <c r="VK2">
-        <v>55</v>
-      </c>
-      <c r="VL2">
-        <v>45</v>
-      </c>
-      <c r="VM2">
-        <v>17</v>
-      </c>
-      <c r="VN2">
-        <v>85</v>
-      </c>
-      <c r="VO2">
-        <v>19</v>
-      </c>
-      <c r="VP2">
-        <v>66</v>
-      </c>
-      <c r="VQ2">
-        <v>63</v>
-      </c>
-      <c r="VR2">
-        <v>112</v>
-      </c>
-      <c r="VS2">
-        <v>1</v>
-      </c>
-      <c r="VT2">
-        <v>4460</v>
-      </c>
-      <c r="VU2">
-        <v>384</v>
-      </c>
-      <c r="VV2">
-        <v>1409</v>
-      </c>
-      <c r="VW2">
-        <v>1899</v>
-      </c>
-      <c r="VX2">
-        <v>1199</v>
-      </c>
-      <c r="VY2">
-        <v>162</v>
-      </c>
-      <c r="VZ2">
-        <v>4460</v>
-      </c>
-      <c r="WA2">
-        <v>2684</v>
-      </c>
-      <c r="WB2">
-        <v>153</v>
-      </c>
-      <c r="WC2">
-        <v>103</v>
-      </c>
-      <c r="WD2">
-        <v>40</v>
-      </c>
-      <c r="WE2">
-        <v>2941</v>
-      </c>
-      <c r="WF2">
-        <v>104</v>
-      </c>
-      <c r="WG2">
-        <v>65</v>
-      </c>
-      <c r="WH2">
-        <v>0</v>
-      </c>
-      <c r="WI2">
-        <v>92</v>
-      </c>
-      <c r="WJ2">
-        <v>62</v>
-      </c>
-      <c r="WK2">
-        <v>17</v>
-      </c>
-      <c r="WL2">
-        <v>0</v>
-      </c>
-      <c r="WM2">
-        <v>0</v>
-      </c>
-      <c r="WN2">
-        <v>0</v>
-      </c>
-      <c r="WO2">
-        <v>413</v>
-      </c>
-      <c r="WP2">
-        <v>114</v>
-      </c>
-      <c r="WQ2">
-        <v>112</v>
-      </c>
-      <c r="WR2">
-        <v>50.4</v>
-      </c>
-      <c r="WS2">
-        <v>24</v>
-      </c>
-      <c r="WT2">
-        <v>49.3</v>
-      </c>
-      <c r="WU2">
-        <v>7</v>
-      </c>
-      <c r="WV2">
-        <v>77</v>
-      </c>
-      <c r="WW2">
-        <v>630</v>
-      </c>
-      <c r="WX2">
+      <c r="XX2">
+        <v>4</v>
+      </c>
+      <c r="XY2">
+        <v>10.5</v>
+      </c>
+      <c r="XZ2">
         <v>5</v>
       </c>
-      <c r="WY2">
-        <v>4</v>
-      </c>
-      <c r="WZ2">
-        <v>0</v>
-      </c>
-      <c r="XA2">
-        <v>0</v>
-      </c>
-      <c r="XB2">
-        <v>11</v>
-      </c>
-      <c r="XC2">
-        <v>0</v>
-      </c>
-      <c r="XD2">
-        <v>0.71</v>
-      </c>
-      <c r="XE2">
-        <v>0.57</v>
-      </c>
-      <c r="XF2">
-        <v>1.29</v>
-      </c>
-      <c r="XG2">
-        <v>0.71</v>
-      </c>
-      <c r="XH2">
-        <v>1.29</v>
-      </c>
-      <c r="XI2">
-        <v>4</v>
-      </c>
-      <c r="XJ2">
-        <v>4</v>
-      </c>
-      <c r="XK2">
-        <v>0.58</v>
-      </c>
-      <c r="XL2">
-        <v>0.58</v>
-      </c>
-      <c r="XM2">
-        <v>7</v>
-      </c>
-      <c r="XN2">
-        <v>7</v>
-      </c>
-      <c r="XO2">
-        <v>630</v>
-      </c>
-      <c r="XP2">
-        <v>11</v>
-      </c>
-      <c r="XQ2">
-        <v>1.57</v>
-      </c>
-      <c r="XR2">
-        <v>32</v>
-      </c>
-      <c r="XS2">
-        <v>21</v>
-      </c>
-      <c r="XT2">
-        <v>65.59999999999999</v>
-      </c>
-      <c r="XU2">
-        <v>2</v>
-      </c>
-      <c r="XV2">
-        <v>1</v>
-      </c>
-      <c r="XW2">
-        <v>4</v>
-      </c>
-      <c r="XX2">
-        <v>1</v>
-      </c>
-      <c r="XY2">
-        <v>14.3</v>
-      </c>
-      <c r="XZ2">
-        <v>0</v>
-      </c>
       <c r="YA2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="YB2">
         <v>0</v>
@@ -6945,346 +6942,346 @@
         <v>0</v>
       </c>
       <c r="YD2">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="YE2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YF2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="YG2">
         <v>0</v>
       </c>
       <c r="YH2">
-        <v>7.8</v>
+        <v>60</v>
       </c>
       <c r="YI2">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="YJ2">
-        <v>-3.2</v>
+        <v>-12</v>
       </c>
       <c r="YK2">
-        <v>-0.46</v>
+        <v>-0.32</v>
       </c>
       <c r="YL2">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="YM2">
-        <v>117</v>
+        <v>643</v>
       </c>
       <c r="YN2">
-        <v>35</v>
+        <v>32.5</v>
       </c>
       <c r="YO2">
-        <v>283</v>
+        <v>1289</v>
       </c>
       <c r="YP2">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="YQ2">
-        <v>35.7</v>
+        <v>40.7</v>
       </c>
       <c r="YR2">
-        <v>35.9</v>
+        <v>36.6</v>
       </c>
       <c r="YS2">
-        <v>44</v>
+        <v>308</v>
       </c>
       <c r="YT2">
-        <v>36.4</v>
+        <v>38.3</v>
       </c>
       <c r="YU2">
-        <v>37.4</v>
+        <v>35.2</v>
       </c>
       <c r="YV2">
-        <v>95</v>
+        <v>528</v>
       </c>
       <c r="YW2">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="YX2">
-        <v>3.2</v>
+        <v>4.5</v>
       </c>
       <c r="YY2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="YZ2">
-        <v>1</v>
+        <v>0.79</v>
       </c>
       <c r="ZA2">
-        <v>18.3</v>
+        <v>13.8</v>
       </c>
       <c r="ZB2">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="ZC2">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="ZD2">
-        <v>31.5</v>
+        <v>30.2</v>
       </c>
       <c r="ZE2">
-        <v>3.29</v>
+        <v>3.53</v>
       </c>
       <c r="ZF2">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="ZG2">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="ZH2">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="ZI2">
-        <v>1</v>
+        <v>-0.1</v>
       </c>
       <c r="ZJ2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="ZK2">
-        <v>2866</v>
+        <v>15167</v>
       </c>
       <c r="ZL2">
-        <v>3610</v>
+        <v>19162</v>
       </c>
       <c r="ZM2">
-        <v>79.40000000000001</v>
+        <v>79.2</v>
       </c>
       <c r="ZN2">
-        <v>51918</v>
+        <v>266542</v>
       </c>
       <c r="ZO2">
-        <v>18904</v>
+        <v>98033</v>
       </c>
       <c r="ZP2">
-        <v>1263</v>
+        <v>6856</v>
       </c>
       <c r="ZQ2">
-        <v>1412</v>
+        <v>7718</v>
       </c>
       <c r="ZR2">
-        <v>89.40000000000001</v>
+        <v>88.8</v>
       </c>
       <c r="ZS2">
-        <v>1221</v>
+        <v>6412</v>
       </c>
       <c r="ZT2">
-        <v>1422</v>
+        <v>7447</v>
       </c>
       <c r="ZU2">
-        <v>85.90000000000001</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="ZV2">
-        <v>323</v>
+        <v>1494</v>
       </c>
       <c r="ZW2">
-        <v>601</v>
+        <v>2927</v>
       </c>
       <c r="ZX2">
-        <v>53.7</v>
+        <v>51</v>
       </c>
       <c r="ZY2">
-        <v>54</v>
+        <v>322</v>
       </c>
       <c r="ZZ2">
-        <v>209</v>
+        <v>1021</v>
       </c>
       <c r="AAA2">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="AAB2">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="AAC2">
-        <v>221</v>
+        <v>1174</v>
       </c>
       <c r="AAD2">
-        <v>3246</v>
+        <v>17161</v>
       </c>
       <c r="AAE2">
-        <v>359</v>
+        <v>1943</v>
       </c>
       <c r="AAF2">
-        <v>105</v>
+        <v>517</v>
       </c>
       <c r="AAG2">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="AAH2">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="AAI2">
-        <v>96</v>
+        <v>571</v>
       </c>
       <c r="AAJ2">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="AAK2">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="AAL2">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="AAM2">
         <v>0</v>
       </c>
       <c r="AAN2">
-        <v>145</v>
+        <v>862</v>
       </c>
       <c r="AAO2">
+        <v>58</v>
+      </c>
+      <c r="AAP2">
+        <v>412</v>
+      </c>
+      <c r="AAQ2">
+        <v>785</v>
+      </c>
+      <c r="AAR2">
+        <v>20.66</v>
+      </c>
+      <c r="AAS2">
+        <v>574</v>
+      </c>
+      <c r="AAT2">
+        <v>67</v>
+      </c>
+      <c r="AAU2">
+        <v>47</v>
+      </c>
+      <c r="AAV2">
+        <v>48</v>
+      </c>
+      <c r="AAW2">
+        <v>76</v>
+      </c>
+      <c r="AAX2">
+        <v>2</v>
+      </c>
+      <c r="AAY2">
+        <v>51</v>
+      </c>
+      <c r="AAZ2">
+        <v>6</v>
+      </c>
+      <c r="ABA2">
         <v>5</v>
       </c>
-      <c r="AAP2">
-        <v>77</v>
-      </c>
-      <c r="AAQ2">
-        <v>127</v>
-      </c>
-      <c r="AAR2">
-        <v>18.14</v>
-      </c>
-      <c r="AAS2">
-        <v>98</v>
-      </c>
-      <c r="AAT2">
+      <c r="ABB2">
+        <v>7</v>
+      </c>
+      <c r="ABC2">
+        <v>2</v>
+      </c>
+      <c r="ABD2">
+        <v>647</v>
+      </c>
+      <c r="ABE2">
+        <v>414</v>
+      </c>
+      <c r="ABF2">
+        <v>330</v>
+      </c>
+      <c r="ABG2">
+        <v>249</v>
+      </c>
+      <c r="ABH2">
+        <v>68</v>
+      </c>
+      <c r="ABI2">
+        <v>457</v>
+      </c>
+      <c r="ABJ2">
+        <v>125</v>
+      </c>
+      <c r="ABK2">
+        <v>332</v>
+      </c>
+      <c r="ABL2">
+        <v>340</v>
+      </c>
+      <c r="ABM2">
+        <v>704</v>
+      </c>
+      <c r="ABN2">
         <v>12</v>
       </c>
-      <c r="AAU2">
-        <v>3</v>
-      </c>
-      <c r="AAV2">
-        <v>3</v>
-      </c>
-      <c r="AAW2">
-        <v>9</v>
-      </c>
-      <c r="AAX2">
-        <v>1.29</v>
-      </c>
-      <c r="AAY2">
-        <v>4</v>
-      </c>
-      <c r="AAZ2">
-        <v>3</v>
-      </c>
-      <c r="ABA2">
-        <v>0</v>
-      </c>
-      <c r="ABB2">
-        <v>0</v>
-      </c>
-      <c r="ABC2">
+      <c r="ABO2">
+        <v>23409</v>
+      </c>
+      <c r="ABP2">
+        <v>2610</v>
+      </c>
+      <c r="ABQ2">
+        <v>8227</v>
+      </c>
+      <c r="ABR2">
+        <v>10686</v>
+      </c>
+      <c r="ABS2">
+        <v>4722</v>
+      </c>
+      <c r="ABT2">
+        <v>611</v>
+      </c>
+      <c r="ABU2">
+        <v>23400</v>
+      </c>
+      <c r="ABV2">
+        <v>12082</v>
+      </c>
+      <c r="ABW2">
+        <v>559</v>
+      </c>
+      <c r="ABX2">
+        <v>407</v>
+      </c>
+      <c r="ABY2">
+        <v>129</v>
+      </c>
+      <c r="ABZ2">
+        <v>14996</v>
+      </c>
+      <c r="ACA2">
+        <v>634</v>
+      </c>
+      <c r="ACB2">
+        <v>322</v>
+      </c>
+      <c r="ACC2">
         <v>1</v>
       </c>
-      <c r="ABD2">
-        <v>98</v>
-      </c>
-      <c r="ABE2">
-        <v>61</v>
-      </c>
-      <c r="ABF2">
-        <v>46</v>
-      </c>
-      <c r="ABG2">
-        <v>44</v>
-      </c>
-      <c r="ABH2">
-        <v>8</v>
-      </c>
-      <c r="ABI2">
-        <v>90</v>
-      </c>
-      <c r="ABJ2">
-        <v>23</v>
-      </c>
-      <c r="ABK2">
-        <v>67</v>
-      </c>
-      <c r="ABL2">
-        <v>60</v>
-      </c>
-      <c r="ABM2">
-        <v>119</v>
-      </c>
-      <c r="ABN2">
-        <v>1</v>
-      </c>
-      <c r="ABO2">
-        <v>4344</v>
-      </c>
-      <c r="ABP2">
-        <v>509</v>
-      </c>
-      <c r="ABQ2">
-        <v>1552</v>
-      </c>
-      <c r="ABR2">
-        <v>1974</v>
-      </c>
-      <c r="ABS2">
-        <v>856</v>
-      </c>
-      <c r="ABT2">
-        <v>99</v>
-      </c>
-      <c r="ABU2">
-        <v>4344</v>
-      </c>
-      <c r="ABV2">
-        <v>2477</v>
-      </c>
-      <c r="ABW2">
-        <v>100</v>
-      </c>
-      <c r="ABX2">
-        <v>77</v>
-      </c>
-      <c r="ABY2">
-        <v>18</v>
-      </c>
-      <c r="ABZ2">
-        <v>2822</v>
-      </c>
-      <c r="ACA2">
-        <v>116</v>
-      </c>
-      <c r="ACB2">
-        <v>63</v>
-      </c>
-      <c r="ACC2">
-        <v>0</v>
-      </c>
       <c r="ACD2">
-        <v>64</v>
+        <v>395</v>
       </c>
       <c r="ACE2">
-        <v>86</v>
+        <v>454</v>
       </c>
       <c r="ACF2">
+        <v>58</v>
+      </c>
+      <c r="ACG2">
+        <v>7</v>
+      </c>
+      <c r="ACH2">
         <v>5</v>
-      </c>
-      <c r="ACG2">
-        <v>0</v>
-      </c>
-      <c r="ACH2">
-        <v>0</v>
       </c>
       <c r="ACI2">
         <v>0</v>
       </c>
       <c r="ACJ2">
-        <v>398</v>
+        <v>1937</v>
       </c>
       <c r="ACK2">
-        <v>112</v>
+        <v>491</v>
       </c>
       <c r="ACL2">
-        <v>114</v>
+        <v>627</v>
       </c>
       <c r="ACM2">
-        <v>49.6</v>
+        <v>43.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>